<commit_message>
Added testcases for contact module and yet to specify the semantics
</commit_message>
<xml_diff>
--- a/src/testdata/CRM.xlsx
+++ b/src/testdata/CRM.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27518"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Ramrasad\qualizeal\playwright_demo\src\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4EE16FCC-9D86-4AA6-A067-7F5A0843827B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAA810F6-C955-4F34-B6FC-7E13709EE964}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{4EE16FCC-9D86-4AA6-A067-7F5A0843827B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2CD80D2-1CA8-4E2A-B3D2-DF62C883F154}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="1" r:id="rId1"/>
+    <sheet name="Contacts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="98">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -195,13 +196,148 @@
   </si>
   <si>
     <t>90000</t>
+  </si>
+  <si>
+    <t>First_name</t>
+  </si>
+  <si>
+    <t>Middle_name</t>
+  </si>
+  <si>
+    <t>Last_name</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Personal_email</t>
+  </si>
+  <si>
+    <t>Channel_type</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Address_street</t>
+  </si>
+  <si>
+    <t>Address_city</t>
+  </si>
+  <si>
+    <t>Address_state</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Phone_Country</t>
+  </si>
+  <si>
+    <t>Phone_Number</t>
+  </si>
+  <si>
+    <t>Phone_Number_Type</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>TC-01</t>
+  </si>
+  <si>
+    <t>Monkey</t>
+  </si>
+  <si>
+    <t>D.</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>Straw hats</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>zoro@gmail.com</t>
+  </si>
+  <si>
+    <t>RANDOM_EMAILID</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>27, Harmada</t>
+  </si>
+  <si>
+    <t>Kota</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>202974</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9453621020 </t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>Administartion</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>business</t>
+  </si>
+  <si>
+    <t>TC-workflow</t>
+  </si>
+  <si>
+    <t>Jagdish</t>
+  </si>
+  <si>
+    <t>Lal</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Jagdish.lal@@manipalcigna.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dmander@rediffmail.com </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,20 +353,97 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -239,10 +452,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -730,4 +954,272 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EAB8E4A-A4DD-418E-BDA0-6B511D42A51B}">
+  <dimension ref="A1:Z3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2:Z3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="19" max="19" width="20.28515625" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" customWidth="1"/>
+    <col min="21" max="21" width="27.28515625" customWidth="1"/>
+    <col min="22" max="22" width="18" customWidth="1"/>
+    <col min="23" max="23" width="22" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" customWidth="1"/>
+    <col min="25" max="25" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15.75">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="15.75">
+      <c r="A2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="16.5">
+      <c r="A3" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{76A20E67-7DB6-44AA-A87A-283AB5C22075}"/>
+    <hyperlink ref="H3" r:id="rId2" display="dmander@" xr:uid="{1D954830-A270-47B8-A339-B1CA0C4A3E2D}"/>
+    <hyperlink ref="I3" r:id="rId3" xr:uid="{642EA648-1EC2-4FBB-9A2D-DBE5B2DE8E5F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>